<commit_message>
Check of some simulations for pressure losses
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/Conditions.xlsx
+++ b/eureca_dhcs/test/input_tests/Conditions.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CEA7B3-AFB7-4F88-AC3D-053D2247D6AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD36AFC1-BF28-4259-BBA8-5D9B6EF47E2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mass_flow" sheetId="1" r:id="rId1"/>
+    <sheet name="nodes_mass_flow" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Node 1</t>
+    <t>Timestep</t>
   </si>
   <si>
-    <t>Node 3</t>
-  </si>
-  <si>
-    <t>Node 5</t>
-  </si>
-  <si>
-    <t>Node 7</t>
+    <t>Node id</t>
   </si>
 </sst>
 </file>
@@ -67,8 +61,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -349,224 +346,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <f>-1*(B2+C2+D2)</f>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>-1*(C3+D3+E3)</f>
         <v>-3</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>-5</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f t="shared" ref="A3:A14" si="0">-1*(B3+C3+D3)</f>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B15" si="0">-1*(C4+D4+E4)</f>
         <v>-3</v>
       </c>
-      <c r="B3">
+      <c r="C4">
         <v>-5</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="B4">
+      <c r="C5">
         <v>-5</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <v>-5</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="B6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="C7">
         <v>-5</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="B7">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="C8">
         <v>-5</v>
       </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="B8">
+      <c r="C9">
         <v>-5</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="B9">
-        <v>-4</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="C10">
+        <v>-4</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="B10">
-        <v>-4</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="C11">
+        <v>-4</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="B11">
-        <v>-4</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="C12">
+        <v>-4</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="B12">
-        <v>-4</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="C13">
+        <v>-4</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="B13">
-        <v>-4</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="C14">
+        <v>-4</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="B14">
-        <v>-4</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
+      <c r="C15">
+        <v>-4</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>